<commit_message>
persistence des resultats de predictions
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22122"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_DC44C33538AF0108512D37DE423C0835E6C6C95E" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{08303BA9-0E4C-4F26-8073-641A7D29917D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,27 +376,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>43735</v>
       </c>
@@ -411,7 +412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>43736</v>
       </c>
@@ -419,7 +420,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>43737</v>
       </c>
@@ -427,7 +428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>43739</v>
       </c>
@@ -435,58 +436,63 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>43740</v>
+      </c>
+      <c r="B6">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -495,8 +501,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b0f053db151659b61f6eea16ec841959">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25f1bff573e4ba7fee595b4d95e5e5cc" ns2:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -536,8 +551,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -626,15 +641,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -642,36 +648,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B125A7-7D23-4D82-B26D-9D593EA4223A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03131341-42B2-46DC-A4C4-C4DD441D0A86}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}"/>
 </file>
</xml_diff>

<commit_message>
test access to Access DB
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22122"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45E226E4-58B9-453E-9F5B-A32D99968E2A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,11 +34,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,27 +376,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,7 +404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>43735</v>
       </c>
@@ -411,7 +412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>43736</v>
       </c>
@@ -419,7 +420,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>43737</v>
       </c>
@@ -427,7 +428,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>43739</v>
       </c>
@@ -435,7 +436,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>43740</v>
       </c>
@@ -443,7 +444,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
         <v>43741</v>
       </c>
@@ -451,52 +452,62 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>43742</v>
+      </c>
+      <c r="B8">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>43743</v>
+      </c>
+      <c r="B9">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -511,17 +522,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b0f053db151659b61f6eea16ec841959">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25f1bff573e4ba7fee595b4d95e5e5cc" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -561,8 +563,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -651,23 +653,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FFC8F9B-4696-4E79-8D7F-50A59CBA2BDC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE020226-4427-431E-9F28-09EF467FC3F1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}"/>
 </file>
</xml_diff>

<commit_message>
zoe: debug sous jupyter, variable explorer jupyter lab pandas-access-db: configuration pour attaquer une base Access
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22204"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{45E226E4-58B9-453E-9F5B-A32D99968E2A}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57FE0CB7-28D7-48AA-AED7-C0BDE3DDBFE4}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,7 +387,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -469,10 +469,20 @@
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>43744</v>
+      </c>
+      <c r="B10">
+        <v>240</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>43745</v>
+      </c>
+      <c r="B11">
+        <v>243</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1"/>
@@ -516,12 +526,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
@@ -653,7 +657,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -662,14 +666,20 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FFC8F9B-4696-4E79-8D7F-50A59CBA2BDC}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FFC8F9B-4696-4E79-8D7F-50A59CBA2BDC}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}"/>
 </file>
</xml_diff>

<commit_message>
week 5 - training neural network
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA52A35E-4E08-42A5-9EBD-50598BE3556B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB5BC624-1C14-4539-AEFD-ED4E52A89752}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +42,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-40C]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,16 +391,16 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,7 +408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43735</v>
       </c>
@@ -417,7 +416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43736</v>
       </c>
@@ -425,7 +424,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43737</v>
       </c>
@@ -433,7 +432,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43739</v>
       </c>
@@ -441,7 +440,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43740</v>
       </c>
@@ -449,7 +448,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43741</v>
       </c>
@@ -457,7 +456,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43742</v>
       </c>
@@ -465,7 +464,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43743</v>
       </c>
@@ -473,7 +472,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43744</v>
       </c>
@@ -481,7 +480,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43745</v>
       </c>
@@ -489,7 +488,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43746</v>
       </c>
@@ -497,7 +496,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43747</v>
       </c>
@@ -505,7 +504,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43748</v>
       </c>
@@ -513,7 +512,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43749</v>
       </c>
@@ -521,7 +520,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43750</v>
       </c>
@@ -529,7 +528,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43751</v>
       </c>
@@ -537,22 +536,32 @@
         <v>439</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43752</v>
+      </c>
+      <c r="B18">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43753</v>
+      </c>
+      <c r="B19">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
@@ -708,13 +717,43 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FFC8F9B-4696-4E79-8D7F-50A59CBA2BDC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FFC8F9B-4696-4E79-8D7F-50A59CBA2BDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fin course week 4 ML Andrew Ng
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{AB5BC624-1C14-4539-AEFD-ED4E52A89752}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_435A78E5709D5C8734C42D2CD6515076B7DD23F8" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{6EF0D21A-9C2D-4285-B8B1-97C3EB67196E}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +553,12 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <v>43754</v>
+      </c>
+      <c r="B20">
+        <v>512</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -570,6 +575,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
@@ -701,22 +721,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FFC8F9B-4696-4E79-8D7F-50A59CBA2BDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -732,28 +761,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
machine learning time series
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="5_{2AF74A12-0847-4AB8-BFBE-679A08320C28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{BA26D1B4-7938-4D91-98FC-AADFFEBD31C8}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="5_{2AF74A12-0847-4AB8-BFBE-679A08320C28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{30DDC8A0-F328-461C-9F19-E59207FC7EFC}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,27 +600,20 @@
         <v>651</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43760</v>
+      </c>
+      <c r="B26">
+        <v>684</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
@@ -752,31 +745,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08737A26-58BF-485A-8D6D-2985C4569B97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -792,4 +776,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
gestion des données manquantes par extrapolation lineaire supporte de plutilples appels au stockage des predictions en conservant à chaque un calcul (le dernier)
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="5_{2AF74A12-0847-4AB8-BFBE-679A08320C28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{30DDC8A0-F328-461C-9F19-E59207FC7EFC}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="5_{2AF74A12-0847-4AB8-BFBE-679A08320C28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C070B43-1DA8-4ED5-87D3-21135EAFC26D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,14 +608,37 @@
         <v>684</v>
       </c>
     </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43761</v>
+      </c>
+      <c r="B27">
+        <v>726</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b0f053db151659b61f6eea16ec841959">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25f1bff573e4ba7fee595b4d95e5e5cc" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -655,8 +678,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -745,35 +768,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08737A26-58BF-485A-8D6D-2985C4569B97}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -787,17 +793,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CF6EE0F-E099-4779-9B67-859483E1DA1D}"/>
 </file>
</xml_diff>

<commit_message>
ajout des 2 graphes de la fin visualisant les kms reels, projection et regression lineaire et l'historique des previsions à 37 mois
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="5_{2AF74A12-0847-4AB8-BFBE-679A08320C28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F13992A-2C6D-4E02-98D1-5366FBF22826}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="5_{2AF74A12-0847-4AB8-BFBE-679A08320C28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{295D1601-18A6-4154-8D40-5CF12E122035}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,12 +624,35 @@
         <v>762</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43763</v>
+      </c>
+      <c r="B29">
+        <v>794</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
@@ -761,23 +784,20 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{322CFC13-A81D-4F6F-843D-3C2C276E3DE8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -789,17 +809,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{322CFC13-A81D-4F6F-843D-3C2C276E3DE8}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
linear classifier et zoe
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michelingroup.sharepoint.com/sites/guiguiperso/Shared Documents/Zoé/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EDACA4F-6C78-4BBF-B2FE-1CB6714CF131}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{549392C7-AE84-441B-BDB7-55E8FB9A1C87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,18 +664,23 @@
         <v>1135</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43782</v>
+      </c>
+      <c r="B34">
+        <v>1170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -811,35 +816,52 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4683461E-8DDB-4A9D-B0FF-D567DCE52EAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4683461E-8DDB-4A9D-B0FF-D567DCE52EAF}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update des plots avec des points "cercles" noirs
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOMF\Sharepoint\MFP Michelin\guigui perso - Documents\Zoé\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\onedrive\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="14_{549392C7-AE84-441B-BDB7-55E8FB9A1C87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{3E01CCEB-C825-48EC-BE3E-2BB5D9AD86F5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47515B3E-7F38-4C5F-A9ED-5C2675149B80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -388,13 +388,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
@@ -680,6 +680,22 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43787</v>
+      </c>
+      <c r="B36">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43795</v>
+      </c>
+      <c r="B37">
+        <v>1485</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -695,8 +711,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="deae782ce3f59c397b974c5d83561ef2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8861602a2a15487ba17460a4c4585d0" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b0f053db151659b61f6eea16ec841959">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25f1bff573e4ba7fee595b4d95e5e5cc" ns2:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -736,8 +752,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -841,20 +857,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{736999D4-1F16-477B-B08D-57465B91F830}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACF281BB-8DB0-4294-961C-F860A6E1872A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>

<commit_message>
feature engineering Signed-off-by: Guillaume Ramelet <guillaume.ramelet@michelin.com>
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\onedrive\MFP Michelin\guigui perso - Documents\Zoé\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michelingroup.sharepoint.com/sites/guiguiperso/Shared Documents/Zoé/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE3328A-59C0-48C9-B181-13C907E78049}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="5_{6C8E882E-806F-47E2-A117-BA7307A717D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{5385AC76-43B2-46F9-A0F3-D2FDE85F3450}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,24 +720,30 @@
         <v>1880</v>
       </c>
     </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43815</v>
+      </c>
+      <c r="B41">
+        <v>2393</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="b0f053db151659b61f6eea16ec841959">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="25f1bff573e4ba7fee595b4d95e5e5cc" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b293a0d2a9486b5dae27f3b98892fd81">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" xmlns:ns3="2475b25d-34f9-4b62-adcb-6f16733d90fb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c50affc3b9283673d7eccf0bdf98037" ns2:_="" ns3:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <xsd:import namespace="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -746,6 +752,8 @@
               <xsd:all>
                 <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -767,6 +775,36 @@
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="2475b25d-34f9-4b62-adcb-6f16733d90fb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="10" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="11" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
     <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
     <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
@@ -776,8 +814,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -867,27 +905,40 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDF53A3D-8784-4667-881E-DD001D13B92E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB18E64C-1C2E-4382-9B88-A5EA9D9C01A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -899,10 +950,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mise à jour Zoé pendant le confinement
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\onedrive\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="5_{6C8E882E-806F-47E2-A117-BA7307A717D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FDDB519-8A4F-472B-9223-077CF1A9CE43}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="5_{6C8E882E-806F-47E2-A117-BA7307A717D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{7501D75C-CE3C-4164-84EA-01947C280CF6}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,18 +752,302 @@
         <v>3180</v>
       </c>
     </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43899</v>
+      </c>
+      <c r="B45">
+        <f t="shared" ref="B45:B74" si="0">B46-1</f>
+        <v>4682</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43900</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>4683</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43901</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>4684</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>43902</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43903</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43904</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>43905</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>4688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43906</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43907</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43908</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43909</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43910</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43911</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43912</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>43913</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>4696</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>43914</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>43915</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>43916</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>4699</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>43917</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>43918</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>4701</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>43919</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>4702</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>43920</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>4703</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>43921</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>4704</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>4705</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>4706</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="0"/>
+        <v>4707</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>43925</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="0"/>
+        <v>4708</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>43926</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="0"/>
+        <v>4709</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="0"/>
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="0"/>
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B75">
+        <f>B76-1</f>
+        <v>4712</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B76">
+        <v>4713</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -932,15 +1216,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -965,18 +1261,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
3 1ers chapitres de create robust workflows
</commit_message>
<xml_diff>
--- a/python-sandbox/zoe/data/kilométrage.xlsx
+++ b/python-sandbox/zoe/data/kilométrage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\onedrive\MFP Michelin\guigui perso - Documents\Zoé\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="5_{6C8E882E-806F-47E2-A117-BA7307A717D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{7501D75C-CE3C-4164-84EA-01947C280CF6}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="5_{6C8E882E-806F-47E2-A117-BA7307A717D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{A94B4CBC-BC8F-4847-A485-E9CA73E97786}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,18 +1039,43 @@
         <v>4713</v>
       </c>
     </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>43941</v>
+      </c>
+      <c r="B77">
+        <v>4726</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>43946</v>
+      </c>
+      <c r="B78">
+        <v>4735</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA6F00A08C77474B8BA8A8E04610D54E" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b293a0d2a9486b5dae27f3b98892fd81">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="49ce4606-b24d-451c-99b6-6262fe2a8a32" xmlns:ns3="2475b25d-34f9-4b62-adcb-6f16733d90fb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1c50affc3b9283673d7eccf0bdf98037" ns2:_="" ns3:_="">
     <xsd:import namespace="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
@@ -1215,33 +1240,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D51D84F5-F9F7-4373-9F3F-D2E0180AF6CD}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="49ce4606-b24d-451c-99b6-6262fe2a8a32"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2475b25d-34f9-4b62-adcb-6f16733d90fb"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB18E64C-1C2E-4382-9B88-A5EA9D9C01A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1258,12 +1282,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{584844D0-90E6-45AB-AFE4-E2943EACAFBB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>